<commit_message>
Restructured the request to isolate from the logic
</commit_message>
<xml_diff>
--- a/hedweb/tests/data/ExcelMultipleSheets.xlsx
+++ b/hedweb/tests/data/ExcelMultipleSheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Research\HEDPython\hed-python\hedweb\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Event code</t>
   </si>
@@ -228,6 +228,21 @@
   </si>
   <si>
     <t>Event/Category/Participant response, (Participant,  (Action/Control Vehicle/Drive/Correct,  Item/Object/Vehicle/Car)), Attribute/Offset</t>
+  </si>
+  <si>
+    <t>Long name</t>
+  </si>
+  <si>
+    <t>PerturbCarToLeft</t>
+  </si>
+  <si>
+    <t>PerturbCarToRight</t>
+  </si>
+  <si>
+    <t>DriverStopsCorrecting</t>
+  </si>
+  <si>
+    <t>DriverStartsToCorrect</t>
   </si>
 </sst>
 </file>
@@ -643,22 +658,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
   <cols>
     <col min="1" max="1" width="15.3828125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.07421875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="57.3828125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.921875" style="2" customWidth="1"/>
-    <col min="5" max="1025" width="8.53515625" customWidth="1"/>
+    <col min="2" max="3" width="23.07421875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="57.3828125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="41.921875" style="2" customWidth="1"/>
+    <col min="6" max="1026" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -666,13 +681,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="58.3">
+    <row r="2" spans="1:5" ht="58.3">
       <c r="A2" s="1">
         <v>251</v>
       </c>
@@ -680,13 +698,16 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58.3">
+    <row r="3" spans="1:5" ht="58.3">
       <c r="A3" s="1">
         <v>252</v>
       </c>
@@ -694,13 +715,16 @@
         <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="47.05" customHeight="1">
+    <row r="4" spans="1:5" ht="47.05" customHeight="1">
       <c r="A4" s="1">
         <v>253</v>
       </c>
@@ -708,13 +732,16 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="58.3">
+    <row r="5" spans="1:5" ht="58.3">
       <c r="A5" s="1">
         <v>254</v>
       </c>
@@ -722,9 +749,12 @@
         <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>